<commit_message>
Update to meeting minutes
</commit_message>
<xml_diff>
--- a/Meeting Minutes/Meeting Minutes.xlsx
+++ b/Meeting Minutes/Meeting Minutes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew Magin\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayde\Documents\OTS-Courier-Services\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11316" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="25-07-2016" sheetId="16" r:id="rId1"/>
@@ -329,9 +329,6 @@
     <t>Discussing changes to website</t>
   </si>
   <si>
-    <t>We then quickly sat down with the clients and discussed a change to the sprint/release planning process. We discussed the removal of story 13 due to it not adding very much business value. And replacing it with a story that assisted the drivers with delivering and picking up packages. Upon discussion they agreed that this was the right move. We proceeded with development</t>
-  </si>
-  <si>
     <t>Story 21</t>
   </si>
   <si>
@@ -372,6 +369,10 @@
   </si>
   <si>
     <t>Complete business letter</t>
+  </si>
+  <si>
+    <t>We then quickly sat down with the clients and discussed a change to the sprint/release planning process. We discussed the removal of story 13 due to it not adding very much business value. And replacing it with a story that assisted the drivers with delivering and picking up packages. Upon discussion they agreed that this was the right move. Similarly, Story 2 was considered too small to be made into its own site and it was decided with the client team that it would be more efficient for this functionality to be added to the assignments page. 
+We proceeded with development</t>
   </si>
 </sst>
 </file>
@@ -761,29 +762,29 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -800,12 +801,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -824,21 +825,21 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -846,7 +847,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -863,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>92</v>
       </c>
@@ -872,55 +873,55 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="3"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
@@ -937,24 +938,24 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -962,7 +963,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -979,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -990,23 +991,23 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>57</v>
@@ -1018,10 +1019,10 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>57</v>
@@ -1033,10 +1034,10 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>57</v>
@@ -1048,9 +1049,9 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>57</v>
@@ -1062,10 +1063,10 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>57</v>
@@ -1077,15 +1078,15 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>18</v>
@@ -1094,20 +1095,20 @@
         <v>42656</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1126,29 +1127,29 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
         <v>104</v>
       </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
@@ -1176,7 +1177,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
@@ -1187,7 +1188,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -1204,20 +1205,20 @@
         <v>42667</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1236,29 +1237,29 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1275,39 +1276,39 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
@@ -1327,21 +1328,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1434,7 +1435,7 @@
         <v>35285</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1453,21 +1454,21 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -1503,7 +1504,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1514,7 +1515,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1531,12 +1532,12 @@
         <v>42597</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1555,21 +1556,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1605,7 +1606,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1616,7 +1617,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>42604</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -1646,7 +1647,7 @@
         <v>42604</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1665,21 +1666,21 @@
       <selection activeCell="A7" sqref="A7:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -1715,7 +1716,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>48</v>
       </c>
@@ -1726,7 +1727,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>52</v>
@@ -1758,7 +1759,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>53</v>
@@ -1773,7 +1774,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>55</v>
       </c>
@@ -1801,7 +1802,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>56</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1834,21 +1835,21 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
@@ -1884,7 +1885,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
@@ -1895,7 +1896,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -1912,20 +1913,20 @@
         <v>42618</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1944,21 +1945,21 @@
       <selection activeCell="E11" sqref="A11:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -1994,7 +1995,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -2011,7 +2012,7 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>74</v>
@@ -2026,7 +2027,7 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>75</v>
@@ -2041,7 +2042,7 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>76</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>77</v>
@@ -2070,15 +2071,15 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -2087,7 +2088,7 @@
         <v>42621</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2106,21 +2107,21 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2145,7 +2146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
@@ -2156,7 +2157,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>65</v>
       </c>
@@ -2167,7 +2168,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -2184,20 +2185,20 @@
         <v>42632</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -2216,21 +2217,21 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.75" customWidth="1"/>
-    <col min="2" max="2" width="55.625" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -2266,7 +2267,7 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>42653</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>86</v>
@@ -2298,7 +2299,7 @@
         <v>42653</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>87</v>
@@ -2313,7 +2314,7 @@
         <v>42653</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>88</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>42653</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>89</v>
@@ -2342,27 +2343,27 @@
         <v>42653</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>

</xml_diff>